<commit_message>
refactor: change TVS diode
change TVS diode
</commit_message>
<xml_diff>
--- a/pcb/myjtag.xlsx
+++ b/pcb/myjtag.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.My_Tech_Studio\1.Project\MyJTAG\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414F83BB-7D50-4369-9070-0B5C8D46945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{746F86FE-6D9B-4D3D-8E46-2312EB154E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{9AA6A76B-1CFD-40F9-B9ED-0F3021F39C0B}"/>
+    <workbookView xWindow="5700" yWindow="0" windowWidth="24885" windowHeight="12285" xr2:uid="{79F4D3F9-90EF-4F02-875C-12F32B101C05}"/>
   </bookViews>
   <sheets>
     <sheet name="myjtag" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="65">
   <si>
     <t>Comment</t>
   </si>
@@ -36,12 +36,12 @@
     <t>Designator</t>
   </si>
   <si>
+    <t>Footprint</t>
+  </si>
+  <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>Footprint</t>
-  </si>
-  <si>
     <t>LibRef</t>
   </si>
   <si>
@@ -87,13 +87,16 @@
     <t>D1, D2</t>
   </si>
   <si>
+    <t>ESD5302</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>SOT23</t>
+  </si>
+  <si>
     <t>PESD5V2S2UT</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>SOT23</t>
   </si>
   <si>
     <t>ESD DIODE</t>
@@ -615,18 +618,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EFEC7F-106E-43B9-8362-75CF0FE9CA96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA8F3C7-C7C0-47EF-8F10-CE5F9EABC61E}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.375" customWidth="1"/>
-    <col min="3" max="3" width="8.75" customWidth="1"/>
-    <col min="4" max="6" width="17.375" customWidth="1"/>
+    <col min="1" max="6" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -656,11 +655,11 @@
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
         <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
@@ -676,11 +675,11 @@
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
         <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>9</v>
@@ -696,11 +695,11 @@
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
         <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
@@ -716,11 +715,11 @@
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
         <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>9</v>
@@ -736,11 +735,11 @@
       <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1">
         <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>17</v>
@@ -756,34 +755,34 @@
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
@@ -791,19 +790,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>10</v>
@@ -811,19 +810,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="1">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>10</v>
@@ -831,39 +830,39 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="1">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1">
         <v>4</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>10</v>
@@ -871,19 +870,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="1">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>10</v>
@@ -891,19 +890,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="1">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>10</v>
@@ -911,19 +910,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="1">
+        <v>47</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1">
         <v>2</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>10</v>
@@ -931,19 +930,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C16" s="1">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>10</v>
@@ -951,39 +950,39 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="1">
+        <v>52</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>10</v>
@@ -991,19 +990,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>10</v>
@@ -1011,22 +1010,22 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="1">
+        <v>62</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>